<commit_message>
j'ai supprimer une image de texte en texte , et j'ai améliorer les alt des iamges
</commit_message>
<xml_diff>
--- a/image présentation/audit SEO.xlsx
+++ b/image présentation/audit SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anais/Site améliorer/image présentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB56A73-9F84-1540-A08D-EBAFD8DA93AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E761B1A-2AD3-0D4C-91E7-B66D5612ABD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{602FDC71-A5EB-C740-9DC9-C5C33D8CF905}"/>
+    <workbookView xWindow="2000" yWindow="660" windowWidth="28800" windowHeight="17500" xr2:uid="{602FDC71-A5EB-C740-9DC9-C5C33D8CF905}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -265,12 +265,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -278,7 +298,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -286,29 +309,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -624,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96F4737-A164-014B-8A27-85AB2D6AAC3E}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A24" sqref="A24:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,321 +661,385 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="5"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="5"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="6"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="5"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="5"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="5"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="5"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="13"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="66">
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
+  <mergeCells count="72">
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
@@ -988,54 +1052,12 @@
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{E35A3E0C-82EA-514F-B15A-046EE57E1A6C}"/>

</xml_diff>

<commit_message>
suppression du lien contact en dessous du titre
</commit_message>
<xml_diff>
--- a/image présentation/audit SEO.xlsx
+++ b/image présentation/audit SEO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anais/Site améliorer/image présentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anais/projet4/image présentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E761B1A-2AD3-0D4C-91E7-B66D5612ABD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4008E5C1-0B21-AE4F-9CD4-A692723A813D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="660" windowWidth="28800" windowHeight="17500" xr2:uid="{602FDC71-A5EB-C740-9DC9-C5C33D8CF905}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{602FDC71-A5EB-C740-9DC9-C5C33D8CF905}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>Catégorie</t>
   </si>
@@ -130,18 +130,12 @@
     <t>les fichier dans le le link html, sans note en min.css mais les fichier dans le site ne sont pas minifier.</t>
   </si>
   <si>
-    <t>liens des partenaire dans le footer</t>
-  </si>
-  <si>
     <t>Enlever les metas, car c'est paas nécessaire pour la regelementation, et les keywords dans le html, ce n'est pas la bonne pratique, il faut cree in fichier css.</t>
   </si>
   <si>
     <t>Pour accueil il n'est pas necessaire car nous somme déjà dans l'accueil et pour le page 2, ce n'est pas logique pourl'utilisateur car page 2 ne défini pas ce que c'est comme page. Mettre juste un lien contact serai la meilleur solution.</t>
   </si>
   <si>
-    <t>il y a beaucoup trop de lien dans le footer, ce qui n'est pas pertinant et au niveaux optimisation ne n'est pas la meilleur pratique.</t>
-  </si>
-  <si>
     <t>j'ai réorganiser les fichier, il avait certain fichier appeler dans les metas qui n'exister pas, donc  je les est renommer.</t>
   </si>
   <si>
@@ -157,9 +151,6 @@
     <t xml:space="preserve">les images ne possede pas tous un alt </t>
   </si>
   <si>
-    <t xml:space="preserve">les liens ne sont pas pertinant au niveau footer, </t>
-  </si>
-  <si>
     <t>https://la-webeuse.com/lien-dans-le-footer/ __ et  https://gloria-project.eu/liens-sitewide/</t>
   </si>
   <si>
@@ -167,9 +158,6 @@
   </si>
   <si>
     <t xml:space="preserve">titre h1, H2 ,H3 </t>
-  </si>
-  <si>
-    <t>https://www.referenseo.com/guide-seo/balises-h1-h2-h3/</t>
   </si>
   <si>
     <t xml:space="preserve">les titres dans le html ne sont pas dans l'ordre  H1, H2 , H3 </t>
@@ -260,54 +248,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -624,20 +635,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96F4737-A164-014B-8A27-85AB2D6AAC3E}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A25"/>
+      <selection activeCell="A16" sqref="A16:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.6640625" customWidth="1"/>
     <col min="2" max="2" width="34.33203125" customWidth="1"/>
-    <col min="3" max="3" width="118.83203125" customWidth="1"/>
-    <col min="4" max="4" width="209.33203125" customWidth="1"/>
+    <col min="3" max="3" width="69.33203125" customWidth="1"/>
+    <col min="4" max="4" width="67.1640625" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" customWidth="1"/>
-    <col min="6" max="6" width="96" customWidth="1"/>
+    <col min="6" max="6" width="44.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -664,334 +675,306 @@
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="13"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="13"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="17" t="s">
+      <c r="D6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="11"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="9" t="s">
+      <c r="D8" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="13"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="9" t="s">
+      <c r="D10" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="13"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="9" t="s">
+      <c r="D12" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="13"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="16"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="12" t="s">
-        <v>42</v>
+      <c r="F14" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="13"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>45</v>
+      <c r="F16" s="15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="16"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="14" t="s">
         <v>23</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="9"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="9"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="14"/>
       <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="A22" s="24"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="72">
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
+  <mergeCells count="66">
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="D2:D3"/>
@@ -1028,36 +1011,30 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F16:F17"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F16:F17"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F20:F21"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{E35A3E0C-82EA-514F-B15A-046EE57E1A6C}"/>
@@ -1067,10 +1044,9 @@
     <hyperlink ref="F8" r:id="rId5" xr:uid="{4686C658-70D0-6243-8C18-F7E2F0C3E307}"/>
     <hyperlink ref="F12" r:id="rId6" xr:uid="{4AB30D74-1C6B-5745-8E9C-69F7688D58DA}"/>
     <hyperlink ref="F14" r:id="rId7" display="https://la-webeuse.com/lien-dans-le-footer/" xr:uid="{934616E8-59BA-134D-A1E9-B32E81042B65}"/>
-    <hyperlink ref="F16" r:id="rId8" xr:uid="{B9219F7C-77D0-B741-A7FF-0B8FA6094CE9}"/>
-    <hyperlink ref="F22" r:id="rId9" xr:uid="{731E0D40-44D5-8246-B4CE-01443FE2BFEF}"/>
-    <hyperlink ref="F18" r:id="rId10" xr:uid="{18DB472A-D9BA-4B40-B648-4801F7F366B1}"/>
-    <hyperlink ref="F20" r:id="rId11" xr:uid="{302684BB-6004-3F48-8922-6AEE3AB8B028}"/>
+    <hyperlink ref="F20" r:id="rId8" xr:uid="{731E0D40-44D5-8246-B4CE-01443FE2BFEF}"/>
+    <hyperlink ref="F16" r:id="rId9" xr:uid="{18DB472A-D9BA-4B40-B648-4801F7F366B1}"/>
+    <hyperlink ref="F18" r:id="rId10" xr:uid="{302684BB-6004-3F48-8922-6AEE3AB8B028}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
envoie du projet 4
</commit_message>
<xml_diff>
--- a/image présentation/audit SEO.xlsx
+++ b/image présentation/audit SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anais/projet4/image présentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4008E5C1-0B21-AE4F-9CD4-A692723A813D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E96179-4874-D743-972C-30A33D753F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{602FDC71-A5EB-C740-9DC9-C5C33D8CF905}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>Catégorie</t>
   </si>
@@ -73,15 +73,9 @@
     <t>SEO ( accessibilite)</t>
   </si>
   <si>
-    <t>meta keywords et keywords dans le html</t>
-  </si>
-  <si>
     <t>SEO (assessibilite et technique)</t>
   </si>
   <si>
-    <t>les meta keywords sont present alors que cela n'est pas necessaire. et les keywords sont dans le html.</t>
-  </si>
-  <si>
     <t>https://www.seo-reference.net/optimisation/black-hat-seo.html</t>
   </si>
   <si>
@@ -130,9 +124,6 @@
     <t>les fichier dans le le link html, sans note en min.css mais les fichier dans le site ne sont pas minifier.</t>
   </si>
   <si>
-    <t>Enlever les metas, car c'est paas nécessaire pour la regelementation, et les keywords dans le html, ce n'est pas la bonne pratique, il faut cree in fichier css.</t>
-  </si>
-  <si>
     <t>Pour accueil il n'est pas necessaire car nous somme déjà dans l'accueil et pour le page 2, ce n'est pas logique pourl'utilisateur car page 2 ne défini pas ce que c'est comme page. Mettre juste un lien contact serai la meilleur solution.</t>
   </si>
   <si>
@@ -185,6 +176,18 @@
   </si>
   <si>
     <t>https://blog.axe-net.fr/hierarchie-balises-h1-h2-hn-referencement/</t>
+  </si>
+  <si>
+    <t>meta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la meta keywords est renseigner et la meta description n'est pas renseigner </t>
+  </si>
+  <si>
+    <t>la meta keywords peux etre laisser ou non, car google ne tient pas compte de cette balise. la meta description est la pour decrire le contenu d'une page web</t>
+  </si>
+  <si>
+    <t>https://optimiz.me/la-balise-meta-keywords/#:~:text=Meta%20keywords%20%3A%20quelle%20d%C3%A9finition%20%3F,certaines%20informations%20(certaines%20m%C3%A9tadonn%C3%A9es).</t>
   </si>
 </sst>
 </file>
@@ -253,72 +256,72 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -635,23 +638,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96F4737-A164-014B-8A27-85AB2D6AAC3E}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A17"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" customWidth="1"/>
-    <col min="3" max="3" width="69.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="56.83203125" customWidth="1"/>
     <col min="4" max="4" width="67.1640625" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
-    <col min="6" max="6" width="44.1640625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -671,351 +675,315 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="13"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="G4" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="16"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="15" t="s">
+      <c r="C12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="18"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="13" t="s">
+      <c r="B14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="E14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="13" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="13"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="15" t="s">
+      <c r="F16" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="17"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="D18" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="16"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="11" t="s">
+      <c r="E18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="13"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C20" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D20" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="3"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="22"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="24"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="66">
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
+  <mergeCells count="67">
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="A16:A17"/>
@@ -1029,12 +997,53 @@
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{E35A3E0C-82EA-514F-B15A-046EE57E1A6C}"/>
@@ -1047,6 +1056,7 @@
     <hyperlink ref="F20" r:id="rId8" xr:uid="{731E0D40-44D5-8246-B4CE-01443FE2BFEF}"/>
     <hyperlink ref="F16" r:id="rId9" xr:uid="{18DB472A-D9BA-4B40-B648-4801F7F366B1}"/>
     <hyperlink ref="F18" r:id="rId10" xr:uid="{302684BB-6004-3F48-8922-6AEE3AB8B028}"/>
+    <hyperlink ref="G4" r:id="rId11" location=":~:text=Meta%20keywords%20%3A%20quelle%20d%C3%A9finition%20%3F,certaines%20informations%20(certaines%20m%C3%A9tadonn%C3%A9es)." xr:uid="{268C9D21-51E2-9E43-8A8D-9BF3BDE3971F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>